<commit_message>
Update Sandwhich gen BYT rep
</commit_message>
<xml_diff>
--- a/zzz_lib/code and data/data/Excel/sandwich_gen_NYT_rep_20250327.xlsx
+++ b/zzz_lib/code and data/data/Excel/sandwich_gen_NYT_rep_20250327.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9eaf80618f9c5e5a/Work Items/TheCareBoard/zzz_lib/code and data/data/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10C66A27-3DE0-4BAC-8E20-32B4C2AAC5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{10C66A27-3DE0-4BAC-8E20-32B4C2AAC5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E5799B8-286C-4357-8983-5CC196149EEB}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{94B09BC3-23A8-483A-BE5C-86794EEC6EAE}"/>
   </bookViews>
@@ -951,11 +951,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2CDB809-6719-4BDD-90F2-B8E874A2CBEF}">
   <dimension ref="A1:J502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>